<commit_message>
"Stored WebElement in object repository and creating on add facility testcase"
</commit_message>
<xml_diff>
--- a/TestData.xlsx
+++ b/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
@@ -16,7 +16,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="20">
   <si>
     <t>Name</t>
   </si>
@@ -68,16 +68,29 @@
     <t>NO.10</t>
   </si>
   <si>
-    <t>Benaglore</t>
-  </si>
-  <si>
     <t>560023</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Tester984</t>
+  </si>
+  <si>
+    <t>tester984@gmail.com</t>
+  </si>
+  <si>
+    <t>7975433984</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -418,19 +431,19 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="21" customWidth="1"/>
-    <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" customWidth="1"/>
-    <col min="9" max="9" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="21.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -479,10 +492,10 @@
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>6</v>
@@ -495,14 +508,30 @@
       <c r="A3" s="2">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2">

</xml_diff>